<commit_message>
new changes to questions 2.3
</commit_message>
<xml_diff>
--- a/assignment2_partC.xlsx
+++ b/assignment2_partC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xanderpoortvliet/Documents/GitHub/Assignment-2-SSO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VanshitaS/Desktop/UVA - Period 1/SSO /SO/Assignment 2/Assignment-2-SSO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BB0A35-64A2-974B-9126-1E70614E6B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58928286-E63B-9F43-B6E0-911A54526714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="32520" windowHeight="20500" activeTab="1" xr2:uid="{F3E6DEA9-584F-C246-93D8-BDE251EAC39F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{F3E6DEA9-584F-C246-93D8-BDE251EAC39F}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise 2.4a" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>Source\destination</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Decision variables y_{ij}</t>
+  </si>
+  <si>
+    <t>Exercise 2.4a</t>
   </si>
 </sst>
 </file>
@@ -242,9 +245,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,13 +256,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -280,15 +279,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
+      <xdr:colOff>233680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123596</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>577273</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>12813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -311,8 +310,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6410960" y="619760"/>
-          <a:ext cx="7772400" cy="2958236"/>
+          <a:off x="5983316" y="643775"/>
+          <a:ext cx="6993775" cy="2694129"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -329,15 +328,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>414867</xdr:colOff>
+      <xdr:colOff>414868</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>108470</xdr:rowOff>
+      <xdr:rowOff>108471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>245534</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>118635</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>65279</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -360,8 +359,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6155267" y="1124470"/>
-          <a:ext cx="15595600" cy="3058165"/>
+          <a:off x="6129868" y="1166804"/>
+          <a:ext cx="9512299" cy="2285142"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -374,7 +373,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -692,8 +691,268 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18661990-AD92-4F4E-8310-14E8A6F29609}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5">
+        <f>SUM(B11:E11)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:F13" si="0">SUM(B12:E12)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5">
+        <f>SUM(B11:B13)</f>
+        <v>10</v>
+      </c>
+      <c r="C14" s="5">
+        <f>SUM(C11:C13)</f>
+        <v>15</v>
+      </c>
+      <c r="D14" s="5">
+        <f>SUM(D11:D13)</f>
+        <v>15</v>
+      </c>
+      <c r="E14" s="5">
+        <f>SUM(E11:E13)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7">
+        <f>SUMPRODUCT(B4:E6,B11:E13)</f>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41D9B12-A7D8-F14E-8113-68D9A026A299}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,7 +961,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -727,62 +986,62 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>20</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>11</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>7</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>9</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>20</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
         <v>14</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>16</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>18</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>15</v>
       </c>
     </row>
@@ -790,16 +1049,16 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
         <v>20</v>
       </c>
     </row>
@@ -829,64 +1088,64 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
         <v>5</v>
       </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>15</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5">
         <f>SUM(B11:E11)</f>
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5">
-        <v>15</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
         <f t="shared" ref="F12:F13" si="0">SUM(B12:E12)</f>
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
         <v>5</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -895,299 +1154,29 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f>SUM(B11:B13)</f>
         <v>10</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f>SUM(C11:C13)</f>
         <v>15</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f>SUM(D11:D13)</f>
         <v>15</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <f>SUM(E11:E13)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8">
-        <f>SUMPRODUCT(B4:E6,B11:E13)</f>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41D9B12-A7D8-F14E-8113-68D9A026A299}">
-  <dimension ref="A1:L35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3">
-        <v>20</v>
-      </c>
-      <c r="F5" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <v>5</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>15</v>
-      </c>
-      <c r="F11" s="6">
-        <f>SUM(B11:E11)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5">
-        <v>15</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" ref="F12:F13" si="0">SUM(B12:E12)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6">
-        <f>SUM(B11:B13)</f>
-        <v>10</v>
-      </c>
-      <c r="C14" s="6">
-        <f>SUM(C11:C13)</f>
-        <v>15</v>
-      </c>
-      <c r="D14" s="6">
-        <f>SUM(D11:D13)</f>
-        <v>15</v>
-      </c>
-      <c r="E14" s="6">
-        <f>SUM(E11:E13)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1204,175 +1193,109 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="8">
         <f>IF(B11&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <f t="shared" ref="C18:E18" si="1">IF(C11&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <f t="shared" ref="B19:E19" si="2">IF(B12&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="10">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8">
         <f t="shared" ref="B20:E20" si="3">IF(B13&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="8">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="7">
         <f>SUMPRODUCT(B4:E6,B11:E13)+100*SUM(B18:E20)</f>
         <v>1060</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G32" s="9"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G33" s="9"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G34" s="9"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>